<commit_message>
Added Phils file for Organization and also updated the combined files.
</commit_message>
<xml_diff>
--- a/OrganisationData/Organisation_MarketingSource_Combined.xlsx
+++ b/OrganisationData/Organisation_MarketingSource_Combined.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ClubCorp\MSS\Marketing Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91DEE629-DE6D-44E0-BE3D-E177D04F7EBC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{762701DE-BE7A-4E4D-9D53-CB73A72660B8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$L$207</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$L$211</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,15 +23,15 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{1A20853C-FC6C-43EC-964B-E3C9D5818D47}" keepAlive="1" name="Query - Organisation_MarketingSource_Combined" description="Connection to the 'Organisation_MarketingSource_Combined' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="Query - Organisation_MarketingSource_Combined" description="Connection to the 'Organisation_MarketingSource_Combined' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Organisation_MarketingSource_Combined;Extended Properties=&quot;&quot;" command="SELECT * FROM [Organisation_MarketingSource_Combined]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2484" uniqueCount="1920">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2494" uniqueCount="1930">
   <si>
     <t>Entity.Code</t>
   </si>
@@ -5797,19 +5791,61 @@
   </si>
   <si>
     <t>https://www.instagram.com/medinagolfcc/</t>
+  </si>
+  <si>
+    <t>01580</t>
+  </si>
+  <si>
+    <t>02285</t>
+  </si>
+  <si>
+    <t>02286</t>
+  </si>
+  <si>
+    <t>02287</t>
+  </si>
+  <si>
+    <t>http://members.clubcorp.com/custom/mss/dashboard_01579-3.jpg</t>
+  </si>
+  <si>
+    <t>http://members.clubcorp.com/custom/mss/dashboard_01579-1.jpg</t>
+  </si>
+  <si>
+    <t>http://members.clubcorp.com/custom/mss/dashboard_01579-4.jpg</t>
+  </si>
+  <si>
+    <t>http://members.clubcorp.com/custom/mss/dashboard_01579-5.jpg</t>
+  </si>
+  <si>
+    <t>35.778642,-78.63999</t>
+  </si>
+  <si>
+    <t>http://images.info.clubcorp.com/EloquaImages/clients/ClubCorpUSA/%7B0eec5dcb-38ea-4213-842e-6d0b410cf5f3%7D_City_Club_Raleigh_Bar_Happy_Hour_Mobile_Hero.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF272525"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1A1A1A"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -5832,9 +5868,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5890,7 +5932,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{0FE6AA2D-DBFA-43DF-89E9-3E772349C90A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="13">
     <queryTableFields count="12">
       <queryTableField id="1" name="Entity.Code" tableColumnId="1"/>
@@ -5911,20 +5953,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44CD292F-6190-45AA-8E54-AA91C72A6D14}" name="Organisation_MarketingSource_Combined" displayName="Organisation_MarketingSource_Combined" ref="A1:L207" tableType="queryTable" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Organisation_MarketingSource_Combined" displayName="Organisation_MarketingSource_Combined" ref="A1:L211" tableType="queryTable" totalsRowShown="0">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{6244CA3A-1C92-4FDE-BF90-7D51C1912563}" uniqueName="1" name="Entity.Code" queryTableFieldId="1" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{254B454B-B32A-489A-8716-A0ACAC373F54}" uniqueName="2" name="Website" queryTableFieldId="2" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{A4FBDE87-EC1E-49DD-8BCA-24F4B7F6D286}" uniqueName="3" name="Twitter" queryTableFieldId="3" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{DEA6FD46-17F6-4BFB-8952-876C563907A6}" uniqueName="4" name="Facebook" queryTableFieldId="4" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{79B14582-BDDE-4AC6-8A83-6B7B9A3434ED}" uniqueName="5" name="Instagram" queryTableFieldId="5" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{F34F573A-04DA-4713-9D22-BDCF42C6BEF0}" uniqueName="6" name="Alternate.Instagram" queryTableFieldId="6" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{1D97F580-6D67-4BDA-BC7F-DBAB3C91595E}" uniqueName="7" name="Club.Location.GeoCode..Rooftop." queryTableFieldId="7" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{7CE819AA-63BE-43E8-8F10-B101A306E806}" uniqueName="8" name="Club.Driving.Directions.GeoCode..Front.door." queryTableFieldId="8" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{DC959A34-754E-45D9-AD43-1EAAFC6830C8}" uniqueName="9" name="Club.Parking.Lot.Latitude" queryTableFieldId="9" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{6EC662C2-5CFC-4CD8-855A-E6A1E1215136}" uniqueName="10" name="Club.Parking.Lot.Longitude" queryTableFieldId="10" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{66B6EBC6-5DA6-4BB1-AE09-F0CBC78160B6}" uniqueName="11" name="Club.Description." queryTableFieldId="11" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{171CB9EC-54AA-48D7-97EC-60621ECDB745}" uniqueName="12" name="Dashboard.Image.URL" queryTableFieldId="12" dataDxfId="0"/>
+    <tableColumn id="1" uniqueName="1" name="Entity.Code" queryTableFieldId="1" dataDxfId="11"/>
+    <tableColumn id="2" uniqueName="2" name="Website" queryTableFieldId="2" dataDxfId="10"/>
+    <tableColumn id="3" uniqueName="3" name="Twitter" queryTableFieldId="3" dataDxfId="9"/>
+    <tableColumn id="4" uniqueName="4" name="Facebook" queryTableFieldId="4" dataDxfId="8"/>
+    <tableColumn id="5" uniqueName="5" name="Instagram" queryTableFieldId="5" dataDxfId="7"/>
+    <tableColumn id="6" uniqueName="6" name="Alternate.Instagram" queryTableFieldId="6" dataDxfId="6"/>
+    <tableColumn id="7" uniqueName="7" name="Club.Location.GeoCode..Rooftop." queryTableFieldId="7" dataDxfId="5"/>
+    <tableColumn id="8" uniqueName="8" name="Club.Driving.Directions.GeoCode..Front.door." queryTableFieldId="8" dataDxfId="4"/>
+    <tableColumn id="9" uniqueName="9" name="Club.Parking.Lot.Latitude" queryTableFieldId="9" dataDxfId="3"/>
+    <tableColumn id="10" uniqueName="10" name="Club.Parking.Lot.Longitude" queryTableFieldId="10" dataDxfId="2"/>
+    <tableColumn id="11" uniqueName="11" name="Club.Description." queryTableFieldId="11" dataDxfId="1"/>
+    <tableColumn id="12" uniqueName="12" name="Dashboard.Image.URL" queryTableFieldId="12" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5973,7 +6015,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -6025,7 +6067,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -6219,19 +6261,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFCE1ED-9A88-4BAD-B6F7-397861D2F7B9}">
-  <dimension ref="A1:L207"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L211"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I18" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="77.7109375" bestFit="1" customWidth="1"/>
@@ -6247,7 +6291,7 @@
     <col min="12" max="12" width="62.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6285,7 +6329,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -6323,7 +6367,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -6361,7 +6405,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
@@ -6399,7 +6443,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>47</v>
       </c>
@@ -6437,7 +6481,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -6475,7 +6519,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>69</v>
       </c>
@@ -6513,7 +6557,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
         <v>80</v>
       </c>
@@ -6551,7 +6595,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
         <v>90</v>
       </c>
@@ -6589,7 +6633,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
         <v>101</v>
       </c>
@@ -6627,7 +6671,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>112</v>
       </c>
@@ -6665,7 +6709,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>123</v>
       </c>
@@ -6703,7 +6747,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
         <v>133</v>
       </c>
@@ -6741,7 +6785,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
         <v>143</v>
       </c>
@@ -6779,7 +6823,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
         <v>153</v>
       </c>
@@ -6817,7 +6861,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
         <v>164</v>
       </c>
@@ -6855,7 +6899,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
         <v>174</v>
       </c>
@@ -6893,7 +6937,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="1" t="s">
         <v>185</v>
       </c>
@@ -6931,7 +6975,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
         <v>196</v>
       </c>
@@ -6969,7 +7013,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
         <v>207</v>
       </c>
@@ -6989,25 +7033,25 @@
         <v>17</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>17</v>
+        <v>1192</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>17</v>
+        <v>1928</v>
+      </c>
+      <c r="I20" s="1">
+        <v>35.778641999999998</v>
+      </c>
+      <c r="J20" s="7">
+        <v>-78.640050000000002</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1196</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
         <v>212</v>
       </c>
@@ -7045,7 +7089,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="1" t="s">
         <v>223</v>
       </c>
@@ -7083,7 +7127,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
         <v>234</v>
       </c>
@@ -7121,7 +7165,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
         <v>245</v>
       </c>
@@ -7159,7 +7203,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="1" t="s">
         <v>255</v>
       </c>
@@ -7197,7 +7241,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="1" t="s">
         <v>262</v>
       </c>
@@ -7235,7 +7279,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="1" t="s">
         <v>272</v>
       </c>
@@ -7273,7 +7317,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
         <v>283</v>
       </c>
@@ -7311,7 +7355,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="1" t="s">
         <v>294</v>
       </c>
@@ -7349,7 +7393,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
         <v>305</v>
       </c>
@@ -7387,7 +7431,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="1" t="s">
         <v>314</v>
       </c>
@@ -7425,7 +7469,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" s="1" t="s">
         <v>325</v>
       </c>
@@ -7463,7 +7507,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" s="1" t="s">
         <v>336</v>
       </c>
@@ -7501,7 +7545,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34" s="1" t="s">
         <v>338</v>
       </c>
@@ -7539,7 +7583,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" s="1" t="s">
         <v>349</v>
       </c>
@@ -7577,7 +7621,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36" s="1" t="s">
         <v>357</v>
       </c>
@@ -7615,7 +7659,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37" s="1" t="s">
         <v>367</v>
       </c>
@@ -7653,7 +7697,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38" s="1" t="s">
         <v>377</v>
       </c>
@@ -7691,7 +7735,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39" s="1" t="s">
         <v>388</v>
       </c>
@@ -7729,7 +7773,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40" s="1" t="s">
         <v>399</v>
       </c>
@@ -7767,7 +7811,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41" s="1" t="s">
         <v>409</v>
       </c>
@@ -7805,7 +7849,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42" s="1" t="s">
         <v>420</v>
       </c>
@@ -7843,7 +7887,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43" s="1" t="s">
         <v>430</v>
       </c>
@@ -7881,7 +7925,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12">
       <c r="A44" s="1" t="s">
         <v>441</v>
       </c>
@@ -7919,7 +7963,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12">
       <c r="A45" s="1" t="s">
         <v>452</v>
       </c>
@@ -7957,7 +8001,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12">
       <c r="A46" s="1" t="s">
         <v>463</v>
       </c>
@@ -7995,7 +8039,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12">
       <c r="A47" s="1" t="s">
         <v>473</v>
       </c>
@@ -8033,7 +8077,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12">
       <c r="A48" s="1" t="s">
         <v>474</v>
       </c>
@@ -8071,7 +8115,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12">
       <c r="A49" s="1" t="s">
         <v>483</v>
       </c>
@@ -8109,7 +8153,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12">
       <c r="A50" s="1" t="s">
         <v>492</v>
       </c>
@@ -8147,7 +8191,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12">
       <c r="A51" s="1" t="s">
         <v>503</v>
       </c>
@@ -8185,7 +8229,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12">
       <c r="A52" s="1" t="s">
         <v>513</v>
       </c>
@@ -8223,7 +8267,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12">
       <c r="A53" s="1" t="s">
         <v>523</v>
       </c>
@@ -8261,7 +8305,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12">
       <c r="A54" s="1" t="s">
         <v>533</v>
       </c>
@@ -8299,7 +8343,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12">
       <c r="A55" s="1" t="s">
         <v>539</v>
       </c>
@@ -8337,7 +8381,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12">
       <c r="A56" s="1" t="s">
         <v>542</v>
       </c>
@@ -8375,7 +8419,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12">
       <c r="A57" s="1" t="s">
         <v>551</v>
       </c>
@@ -8413,7 +8457,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12">
       <c r="A58" s="1" t="s">
         <v>562</v>
       </c>
@@ -8451,7 +8495,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12">
       <c r="A59" s="1" t="s">
         <v>573</v>
       </c>
@@ -8489,7 +8533,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12">
       <c r="A60" s="1" t="s">
         <v>585</v>
       </c>
@@ -8527,7 +8571,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12">
       <c r="A61" s="1" t="s">
         <v>596</v>
       </c>
@@ -8565,7 +8609,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12">
       <c r="A62" s="1" t="s">
         <v>607</v>
       </c>
@@ -8603,7 +8647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12">
       <c r="A63" s="1" t="s">
         <v>608</v>
       </c>
@@ -8641,7 +8685,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12">
       <c r="A64" s="1" t="s">
         <v>617</v>
       </c>
@@ -8679,7 +8723,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12">
       <c r="A65" s="1" t="s">
         <v>628</v>
       </c>
@@ -8717,7 +8761,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12">
       <c r="A66" s="1" t="s">
         <v>639</v>
       </c>
@@ -8755,7 +8799,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12">
       <c r="A67" s="1" t="s">
         <v>649</v>
       </c>
@@ -8793,7 +8837,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12">
       <c r="A68" s="1" t="s">
         <v>660</v>
       </c>
@@ -8831,7 +8875,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12">
       <c r="A69" s="1" t="s">
         <v>663</v>
       </c>
@@ -8869,7 +8913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12">
       <c r="A70" s="1" t="s">
         <v>665</v>
       </c>
@@ -8907,7 +8951,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12">
       <c r="A71" s="1" t="s">
         <v>677</v>
       </c>
@@ -8945,7 +8989,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12">
       <c r="A72" s="1" t="s">
         <v>688</v>
       </c>
@@ -8983,7 +9027,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12">
       <c r="A73" s="1" t="s">
         <v>698</v>
       </c>
@@ -9021,7 +9065,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12">
       <c r="A74" s="1" t="s">
         <v>709</v>
       </c>
@@ -9059,7 +9103,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12">
       <c r="A75" s="1" t="s">
         <v>719</v>
       </c>
@@ -9097,7 +9141,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12">
       <c r="A76" s="1" t="s">
         <v>730</v>
       </c>
@@ -9135,7 +9179,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12">
       <c r="A77" s="1" t="s">
         <v>740</v>
       </c>
@@ -9173,7 +9217,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12">
       <c r="A78" s="1" t="s">
         <v>743</v>
       </c>
@@ -9211,7 +9255,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12">
       <c r="A79" s="1" t="s">
         <v>754</v>
       </c>
@@ -9249,7 +9293,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12">
       <c r="A80" s="1" t="s">
         <v>765</v>
       </c>
@@ -9287,7 +9331,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12">
       <c r="A81" s="1" t="s">
         <v>773</v>
       </c>
@@ -9325,7 +9369,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12">
       <c r="A82" s="1" t="s">
         <v>783</v>
       </c>
@@ -9363,7 +9407,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12">
       <c r="A83" s="1" t="s">
         <v>794</v>
       </c>
@@ -9401,7 +9445,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12">
       <c r="A84" s="1" t="s">
         <v>803</v>
       </c>
@@ -9439,7 +9483,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12">
       <c r="A85" s="1" t="s">
         <v>814</v>
       </c>
@@ -9477,7 +9521,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12">
       <c r="A86" s="1" t="s">
         <v>824</v>
       </c>
@@ -9515,7 +9559,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12">
       <c r="A87" s="1" t="s">
         <v>835</v>
       </c>
@@ -9553,7 +9597,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12">
       <c r="A88" s="1" t="s">
         <v>844</v>
       </c>
@@ -9591,7 +9635,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12">
       <c r="A89" s="1" t="s">
         <v>856</v>
       </c>
@@ -9629,7 +9673,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12">
       <c r="A90" s="1" t="s">
         <v>865</v>
       </c>
@@ -9667,7 +9711,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12">
       <c r="A91" s="1" t="s">
         <v>875</v>
       </c>
@@ -9705,7 +9749,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12">
       <c r="A92" s="1" t="s">
         <v>884</v>
       </c>
@@ -9743,7 +9787,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12">
       <c r="A93" s="1" t="s">
         <v>885</v>
       </c>
@@ -9781,7 +9825,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12">
       <c r="A94" s="1" t="s">
         <v>896</v>
       </c>
@@ -9819,7 +9863,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12">
       <c r="A95" s="1" t="s">
         <v>907</v>
       </c>
@@ -9857,7 +9901,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12">
       <c r="A96" s="1" t="s">
         <v>918</v>
       </c>
@@ -9895,7 +9939,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12">
       <c r="A97" s="1" t="s">
         <v>927</v>
       </c>
@@ -9933,7 +9977,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12">
       <c r="A98" s="1" t="s">
         <v>938</v>
       </c>
@@ -9971,7 +10015,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12">
       <c r="A99" s="1" t="s">
         <v>949</v>
       </c>
@@ -10009,7 +10053,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12">
       <c r="A100" s="1" t="s">
         <v>961</v>
       </c>
@@ -10047,7 +10091,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12">
       <c r="A101" s="1" t="s">
         <v>971</v>
       </c>
@@ -10085,7 +10129,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12">
       <c r="A102" s="1" t="s">
         <v>980</v>
       </c>
@@ -10123,7 +10167,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12">
       <c r="A103" s="1" t="s">
         <v>989</v>
       </c>
@@ -10161,7 +10205,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12">
       <c r="A104" s="1" t="s">
         <v>1000</v>
       </c>
@@ -10199,7 +10243,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12">
       <c r="A105" s="1" t="s">
         <v>1011</v>
       </c>
@@ -10237,7 +10281,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12">
       <c r="A106" s="1" t="s">
         <v>1022</v>
       </c>
@@ -10275,7 +10319,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12">
       <c r="A107" s="1" t="s">
         <v>1033</v>
       </c>
@@ -10313,7 +10357,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12">
       <c r="A108" s="1" t="s">
         <v>1044</v>
       </c>
@@ -10351,7 +10395,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12">
       <c r="A109" s="1" t="s">
         <v>1053</v>
       </c>
@@ -10389,7 +10433,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12">
       <c r="A110" s="1" t="s">
         <v>1056</v>
       </c>
@@ -10427,7 +10471,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12">
       <c r="A111" s="1" t="s">
         <v>1067</v>
       </c>
@@ -10465,7 +10509,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12">
       <c r="A112" s="1" t="s">
         <v>1076</v>
       </c>
@@ -10503,7 +10547,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12">
       <c r="A113" s="1" t="s">
         <v>1087</v>
       </c>
@@ -10541,7 +10585,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12">
       <c r="A114" s="1" t="s">
         <v>1098</v>
       </c>
@@ -10579,7 +10623,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12">
       <c r="A115" s="1" t="s">
         <v>1109</v>
       </c>
@@ -10617,7 +10661,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12">
       <c r="A116" s="1" t="s">
         <v>1118</v>
       </c>
@@ -10655,7 +10699,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12">
       <c r="A117" s="1" t="s">
         <v>1127</v>
       </c>
@@ -10693,7 +10737,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12">
       <c r="A118" s="1" t="s">
         <v>1139</v>
       </c>
@@ -10731,7 +10775,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12">
       <c r="A119" s="1" t="s">
         <v>1147</v>
       </c>
@@ -10769,7 +10813,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12">
       <c r="A120" s="1" t="s">
         <v>1157</v>
       </c>
@@ -10807,7 +10851,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12">
       <c r="A121" s="1" t="s">
         <v>1169</v>
       </c>
@@ -10845,7 +10889,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12">
       <c r="A122" s="1" t="s">
         <v>1180</v>
       </c>
@@ -10883,7 +10927,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12">
       <c r="A123" s="1" t="s">
         <v>1191</v>
       </c>
@@ -10921,7 +10965,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12">
       <c r="A124" s="1" t="s">
         <v>1198</v>
       </c>
@@ -10959,7 +11003,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12">
       <c r="A125" s="1" t="s">
         <v>1209</v>
       </c>
@@ -10997,7 +11041,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12">
       <c r="A126" s="1" t="s">
         <v>1219</v>
       </c>
@@ -11035,7 +11079,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12">
       <c r="A127" s="1" t="s">
         <v>1230</v>
       </c>
@@ -11073,7 +11117,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12">
       <c r="A128" s="1" t="s">
         <v>1241</v>
       </c>
@@ -11111,7 +11155,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12">
       <c r="A129" s="1" t="s">
         <v>1251</v>
       </c>
@@ -11149,7 +11193,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12">
       <c r="A130" s="1" t="s">
         <v>1261</v>
       </c>
@@ -11187,7 +11231,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12">
       <c r="A131" s="1" t="s">
         <v>1270</v>
       </c>
@@ -11225,7 +11269,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12">
       <c r="A132" s="1" t="s">
         <v>1280</v>
       </c>
@@ -11263,7 +11307,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12">
       <c r="A133" s="1" t="s">
         <v>1291</v>
       </c>
@@ -11301,7 +11345,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12">
       <c r="A134" s="1" t="s">
         <v>1302</v>
       </c>
@@ -11339,7 +11383,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12">
       <c r="A135" s="1" t="s">
         <v>1308</v>
       </c>
@@ -11377,7 +11421,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12">
       <c r="A136" s="1" t="s">
         <v>1314</v>
       </c>
@@ -11415,7 +11459,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12">
       <c r="A137" s="1" t="s">
         <v>1320</v>
       </c>
@@ -11453,7 +11497,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12">
       <c r="A138" s="1" t="s">
         <v>1331</v>
       </c>
@@ -11491,7 +11535,7 @@
         <v>1341</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12">
       <c r="A139" s="1" t="s">
         <v>1342</v>
       </c>
@@ -11529,7 +11573,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12">
       <c r="A140" s="1" t="s">
         <v>1353</v>
       </c>
@@ -11567,7 +11611,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12">
       <c r="A141" s="1" t="s">
         <v>1364</v>
       </c>
@@ -11605,7 +11649,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12">
       <c r="A142" s="1" t="s">
         <v>1375</v>
       </c>
@@ -11643,7 +11687,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12">
       <c r="A143" s="1" t="s">
         <v>1384</v>
       </c>
@@ -11681,7 +11725,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12">
       <c r="A144" s="1" t="s">
         <v>1395</v>
       </c>
@@ -11719,7 +11763,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12">
       <c r="A145" s="1" t="s">
         <v>1406</v>
       </c>
@@ -11757,7 +11801,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12">
       <c r="A146" s="1" t="s">
         <v>1417</v>
       </c>
@@ -11795,7 +11839,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12">
       <c r="A147" s="1" t="s">
         <v>1419</v>
       </c>
@@ -11833,7 +11877,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12">
       <c r="A148" s="1" t="s">
         <v>1430</v>
       </c>
@@ -11871,7 +11915,7 @@
         <v>1441</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12">
       <c r="A149" s="1" t="s">
         <v>1442</v>
       </c>
@@ -11909,7 +11953,7 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12">
       <c r="A150" s="1" t="s">
         <v>1452</v>
       </c>
@@ -11947,7 +11991,7 @@
         <v>1462</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12">
       <c r="A151" s="1" t="s">
         <v>1463</v>
       </c>
@@ -11985,7 +12029,7 @@
         <v>1468</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12">
       <c r="A152" s="1" t="s">
         <v>1469</v>
       </c>
@@ -12023,7 +12067,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12">
       <c r="A153" s="1" t="s">
         <v>1479</v>
       </c>
@@ -12061,7 +12105,7 @@
         <v>1489</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12">
       <c r="A154" s="1" t="s">
         <v>1490</v>
       </c>
@@ -12099,7 +12143,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12">
       <c r="A155" s="1" t="s">
         <v>1500</v>
       </c>
@@ -12137,7 +12181,7 @@
         <v>1509</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12">
       <c r="A156" s="1" t="s">
         <v>1510</v>
       </c>
@@ -12175,7 +12219,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12">
       <c r="A157" s="1" t="s">
         <v>1521</v>
       </c>
@@ -12213,7 +12257,7 @@
         <v>1531</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12">
       <c r="A158" s="1" t="s">
         <v>1532</v>
       </c>
@@ -12251,7 +12295,7 @@
         <v>1541</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12">
       <c r="A159" s="1" t="s">
         <v>1542</v>
       </c>
@@ -12289,7 +12333,7 @@
         <v>1551</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12">
       <c r="A160" s="1" t="s">
         <v>1552</v>
       </c>
@@ -12327,7 +12371,7 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12">
       <c r="A161" s="1" t="s">
         <v>1561</v>
       </c>
@@ -12365,7 +12409,7 @@
         <v>1571</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12">
       <c r="A162" s="1" t="s">
         <v>1572</v>
       </c>
@@ -12403,7 +12447,7 @@
         <v>1582</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12">
       <c r="A163" s="1" t="s">
         <v>1583</v>
       </c>
@@ -12441,7 +12485,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12">
       <c r="A164" s="1" t="s">
         <v>1591</v>
       </c>
@@ -12479,7 +12523,7 @@
         <v>1598</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12">
       <c r="A165" s="1" t="s">
         <v>1599</v>
       </c>
@@ -12517,7 +12561,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12">
       <c r="A166" s="1" t="s">
         <v>1608</v>
       </c>
@@ -12555,7 +12599,7 @@
         <v>1614</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12">
       <c r="A167" s="1" t="s">
         <v>1615</v>
       </c>
@@ -12593,7 +12637,7 @@
         <v>1623</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12">
       <c r="A168" s="1" t="s">
         <v>1624</v>
       </c>
@@ -12631,7 +12675,7 @@
         <v>1629</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12">
       <c r="A169" s="1" t="s">
         <v>1630</v>
       </c>
@@ -12669,7 +12713,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12">
       <c r="A170" s="1" t="s">
         <v>1636</v>
       </c>
@@ -12707,7 +12751,7 @@
         <v>1645</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12">
       <c r="A171" s="1" t="s">
         <v>1646</v>
       </c>
@@ -12745,7 +12789,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12">
       <c r="A172" s="1" t="s">
         <v>1656</v>
       </c>
@@ -12783,7 +12827,7 @@
         <v>1664</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12">
       <c r="A173" s="1" t="s">
         <v>1665</v>
       </c>
@@ -12821,7 +12865,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12">
       <c r="A174" s="1" t="s">
         <v>1668</v>
       </c>
@@ -12859,7 +12903,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12">
       <c r="A175" s="1" t="s">
         <v>1671</v>
       </c>
@@ -12897,7 +12941,7 @@
         <v>1677</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12">
       <c r="A176" s="1" t="s">
         <v>1678</v>
       </c>
@@ -12935,7 +12979,7 @@
         <v>1686</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12">
       <c r="A177" s="1" t="s">
         <v>1687</v>
       </c>
@@ -12973,7 +13017,7 @@
         <v>1692</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12">
       <c r="A178" s="1" t="s">
         <v>1693</v>
       </c>
@@ -13011,7 +13055,7 @@
         <v>1698</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12">
       <c r="A179" s="1" t="s">
         <v>1699</v>
       </c>
@@ -13049,7 +13093,7 @@
         <v>1704</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12">
       <c r="A180" s="1" t="s">
         <v>1705</v>
       </c>
@@ -13087,7 +13131,7 @@
         <v>1713</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12">
       <c r="A181" s="1" t="s">
         <v>1714</v>
       </c>
@@ -13125,7 +13169,7 @@
         <v>1724</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12">
       <c r="A182" s="1" t="s">
         <v>1725</v>
       </c>
@@ -13163,7 +13207,7 @@
         <v>1735</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12">
       <c r="A183" s="1" t="s">
         <v>1736</v>
       </c>
@@ -13201,7 +13245,7 @@
         <v>1744</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12">
       <c r="A184" s="1" t="s">
         <v>1745</v>
       </c>
@@ -13239,7 +13283,7 @@
         <v>1755</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12">
       <c r="A185" s="1" t="s">
         <v>1756</v>
       </c>
@@ -13277,7 +13321,7 @@
         <v>1761</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12">
       <c r="A186" s="1" t="s">
         <v>1762</v>
       </c>
@@ -13315,7 +13359,7 @@
         <v>1772</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12">
       <c r="A187" s="1" t="s">
         <v>1773</v>
       </c>
@@ -13353,7 +13397,7 @@
         <v>1782</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12">
       <c r="A188" s="1" t="s">
         <v>1783</v>
       </c>
@@ -13391,7 +13435,7 @@
         <v>1792</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12">
       <c r="A189" s="1" t="s">
         <v>1793</v>
       </c>
@@ -13429,7 +13473,7 @@
         <v>1798</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12">
       <c r="A190" s="1" t="s">
         <v>1799</v>
       </c>
@@ -13467,7 +13511,7 @@
         <v>1804</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12">
       <c r="A191" s="1" t="s">
         <v>1805</v>
       </c>
@@ -13505,7 +13549,7 @@
         <v>1814</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12">
       <c r="A192" s="1" t="s">
         <v>1815</v>
       </c>
@@ -13543,7 +13587,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12">
       <c r="A193" s="1" t="s">
         <v>1822</v>
       </c>
@@ -13581,7 +13625,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12">
       <c r="A194" s="1" t="s">
         <v>1825</v>
       </c>
@@ -13619,7 +13663,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12">
       <c r="A195" s="1" t="s">
         <v>1826</v>
       </c>
@@ -13657,7 +13701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12">
       <c r="A196" s="1" t="s">
         <v>1829</v>
       </c>
@@ -13695,7 +13739,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12">
       <c r="A197" s="1" t="s">
         <v>1831</v>
       </c>
@@ -13733,7 +13777,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12">
       <c r="A198" s="1" t="s">
         <v>1841</v>
       </c>
@@ -13771,7 +13815,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12">
       <c r="A199" s="1" t="s">
         <v>1843</v>
       </c>
@@ -13809,7 +13853,7 @@
         <v>1852</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12">
       <c r="A200" s="1" t="s">
         <v>1853</v>
       </c>
@@ -13847,7 +13891,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12">
       <c r="A201" s="1" t="s">
         <v>1864</v>
       </c>
@@ -13885,7 +13929,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12">
       <c r="A202" s="1" t="s">
         <v>1865</v>
       </c>
@@ -13923,7 +13967,7 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12">
       <c r="A203" s="1" t="s">
         <v>1876</v>
       </c>
@@ -13961,7 +14005,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12">
       <c r="A204" s="1" t="s">
         <v>1887</v>
       </c>
@@ -13999,7 +14043,7 @@
         <v>1897</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12">
       <c r="A205" s="1" t="s">
         <v>1898</v>
       </c>
@@ -14037,7 +14081,7 @@
         <v>1906</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12">
       <c r="A206" s="1" t="s">
         <v>1907</v>
       </c>
@@ -14075,7 +14119,7 @@
         <v>1916</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12">
       <c r="A207" s="1" t="s">
         <v>1917</v>
       </c>
@@ -14113,21 +14157,118 @@
         <v>17</v>
       </c>
     </row>
+    <row r="208" spans="1:12" ht="15.75">
+      <c r="A208" s="3" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B208" s="1"/>
+      <c r="C208" s="1"/>
+      <c r="D208" s="1"/>
+      <c r="E208" s="1"/>
+      <c r="F208" s="1"/>
+      <c r="G208" s="1"/>
+      <c r="H208" s="1"/>
+      <c r="I208" s="5">
+        <v>30.364485003256</v>
+      </c>
+      <c r="J208" s="5">
+        <v>-97.993275215912902</v>
+      </c>
+      <c r="K208" s="6" t="s">
+        <v>1074</v>
+      </c>
+      <c r="L208" t="s">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" ht="15.75">
+      <c r="A209" s="3" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B209" s="1"/>
+      <c r="C209" s="1"/>
+      <c r="D209" s="1"/>
+      <c r="E209" s="1"/>
+      <c r="F209" s="1"/>
+      <c r="G209" s="1"/>
+      <c r="H209" s="1"/>
+      <c r="I209" s="5">
+        <v>30.338731858635999</v>
+      </c>
+      <c r="J209" s="5">
+        <v>-97.982731461525006</v>
+      </c>
+      <c r="K209" s="6" t="s">
+        <v>1074</v>
+      </c>
+      <c r="L209" t="s">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" ht="15.75">
+      <c r="A210" s="3" t="s">
+        <v>1922</v>
+      </c>
+      <c r="B210" s="1"/>
+      <c r="C210" s="1"/>
+      <c r="D210" s="1"/>
+      <c r="E210" s="1"/>
+      <c r="F210" s="1"/>
+      <c r="G210" s="1"/>
+      <c r="H210" s="1"/>
+      <c r="I210" s="5">
+        <v>30.350715320971499</v>
+      </c>
+      <c r="J210" s="5">
+        <v>-97.996799647808103</v>
+      </c>
+      <c r="K210" s="6" t="s">
+        <v>1074</v>
+      </c>
+      <c r="L210" t="s">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" ht="15.75">
+      <c r="A211" s="4" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B211" s="2"/>
+      <c r="C211" s="2"/>
+      <c r="D211" s="2"/>
+      <c r="E211" s="2"/>
+      <c r="F211" s="2"/>
+      <c r="G211" s="2"/>
+      <c r="H211" s="2"/>
+      <c r="I211" s="5">
+        <v>30.3591169894299</v>
+      </c>
+      <c r="J211" s="5">
+        <v>-97.967374473810196</v>
+      </c>
+      <c r="K211" s="6" t="s">
+        <v>1074</v>
+      </c>
+      <c r="L211" t="s">
+        <v>1927</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E923E94-8CB9-4E5F-A561-8FDF4B221647}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>